<commit_message>
Add table with TCAs
</commit_message>
<xml_diff>
--- a/doc/tc_algorithm_repository.xlsx
+++ b/doc/tc_algorithm_repository.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithms" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>Topology</t>
+  </si>
+  <si>
+    <t>FETC</t>
+  </si>
+  <si>
+    <t>Fair and Energyefficient TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Topology Control Protocol for 2D Poisson Distributed Wireless Sensor Networks http://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=5136711 </t>
   </si>
 </sst>
 </file>
@@ -628,31 +637,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -687,7 +696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -710,7 +719,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -730,7 +739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -750,7 +759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -764,7 +773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -778,7 +787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -792,7 +801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -809,7 +818,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -830,7 +839,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -843,7 +852,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -857,7 +866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -868,7 +877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -892,7 +901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -913,6 +922,20 @@
       </c>
       <c r="K14" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -933,13 +956,13 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="125.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="125.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -950,12 +973,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -966,7 +989,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -974,7 +997,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -982,7 +1005,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -990,7 +1013,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -998,7 +1021,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>57</v>
       </c>

</xml_diff>